<commit_message>
Kyle add logarithmic return
</commit_message>
<xml_diff>
--- a/Collab_3.1.1.xlsx
+++ b/Collab_3.1.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/nghia002_e_ntu_edu_sg/Documents/OneDrive/Finance/WQU/MScFE 610 Econometrics/Week 3 Univariate Time Series Models/econometrics_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8390E162-4F96-AB43-9C75-5C11CA69C1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{A81ACAF0-62F2-F145-BCC5-BF5C28A5F82B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JPM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="10" uniqueCount="10">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -64,11 +64,14 @@
   <si>
     <t>Daily return</t>
   </si>
+  <si>
+    <t>Daily logarithmic return</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2490,21 +2493,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K232"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="K236" sqref="K236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2529,8 +2532,11 @@
       <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="d">
         <v>2018-01-31</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>13141400</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="d">
         <v>2018-02-01</v>
       </c>
@@ -2579,8 +2585,12 @@
         <f>(F3/F2)-1</f>
         <v>1.0374371535315507E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <f>LN(F3/F2)</f>
+        <v>1.0320927060360859E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="d">
         <v>2018-02-02</v>
       </c>
@@ -2606,8 +2616,12 @@
         <f t="shared" ref="K4:K67" si="0">(F4/F3)-1</f>
         <v>-2.2161369242984841E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <f t="shared" ref="L4:L67" si="1">LN(F4/F3)</f>
+        <v>-2.241062178714541E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="d">
         <v>2018-02-05</v>
       </c>
@@ -2633,8 +2647,12 @@
         <f t="shared" si="0"/>
         <v>-4.7952357240604093E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>-4.9140200527644902E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="d">
         <v>2018-02-06</v>
       </c>
@@ -2660,8 +2678,12 @@
         <f t="shared" si="0"/>
         <v>3.0422833594320853E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>2.9969236054801045E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="d">
         <v>2018-02-07</v>
       </c>
@@ -2687,8 +2709,12 @@
         <f t="shared" si="0"/>
         <v>6.7790183071771981E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>6.7561440809160052E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="d">
         <v>2018-02-08</v>
       </c>
@@ -2714,8 +2740,12 @@
         <f t="shared" si="0"/>
         <v>-4.4210206546455577E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>-4.5217271432922757E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="d">
         <v>2018-02-09</v>
       </c>
@@ -2741,8 +2771,12 @@
         <f t="shared" si="0"/>
         <v>2.0022238224919331E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1.9824429239809073E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="d">
         <v>2018-02-12</v>
       </c>
@@ -2768,8 +2802,12 @@
         <f t="shared" si="0"/>
         <v>1.5448863605186824E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1.5330744891709071E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="d">
         <v>2018-02-13</v>
       </c>
@@ -2795,8 +2833,12 @@
         <f t="shared" si="0"/>
         <v>6.1751737854471855E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>6.1561855302297609E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="d">
         <v>2018-02-14</v>
       </c>
@@ -2822,8 +2864,12 @@
         <f t="shared" si="0"/>
         <v>2.3125494524860013E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>2.286215249059571E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="d">
         <v>2018-02-15</v>
       </c>
@@ -2849,8 +2895,12 @@
         <f t="shared" si="0"/>
         <v>4.1728093974697789E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>4.1641273722469972E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="d">
         <v>2018-02-16</v>
       </c>
@@ -2876,8 +2926,12 @@
         <f t="shared" si="0"/>
         <v>-7.185467466133022E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>-7.2114072719320528E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="d">
         <v>2018-02-20</v>
       </c>
@@ -2903,8 +2957,12 @@
         <f t="shared" si="0"/>
         <v>2.6152220739672494E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>2.6148801642524646E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="d">
         <v>2018-02-21</v>
       </c>
@@ -2930,8 +2988,12 @@
         <f t="shared" si="0"/>
         <v>4.184441107472292E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>4.1757106799475757E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="d">
         <v>2018-02-22</v>
       </c>
@@ -2957,8 +3019,12 @@
         <f t="shared" si="0"/>
         <v>-1.8230023450415134E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>-1.8246660360657519E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="d">
         <v>2018-02-23</v>
       </c>
@@ -2984,8 +3050,12 @@
         <f t="shared" si="0"/>
         <v>2.0264402656204439E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>2.0061811995320037E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="d">
         <v>2018-02-26</v>
       </c>
@@ -3011,8 +3081,12 @@
         <f t="shared" si="0"/>
         <v>1.2445598566037219E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>1.236878874373787E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="d">
         <v>2018-02-27</v>
       </c>
@@ -3038,8 +3112,12 @@
         <f t="shared" si="0"/>
         <v>-1.1871714006846057E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>-1.1942745540662247E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="d">
         <v>2018-02-28</v>
       </c>
@@ -3065,8 +3143,12 @@
         <f t="shared" si="0"/>
         <v>-1.584855568505894E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>-1.597548694819672E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="d">
         <v>2018-03-01</v>
       </c>
@@ -3092,8 +3174,12 @@
         <f t="shared" si="0"/>
         <v>-1.792210285276119E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>-1.8084648776544181E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="d">
         <v>2018-03-02</v>
       </c>
@@ -3119,8 +3205,12 @@
         <f t="shared" si="0"/>
         <v>-9.6985831711238202E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>-9.7032893400242706E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="d">
         <v>2018-03-05</v>
       </c>
@@ -3146,8 +3236,12 @@
         <f t="shared" si="0"/>
         <v>1.5354804545662848E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>1.5238112540225406E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="d">
         <v>2018-03-06</v>
       </c>
@@ -3173,8 +3267,12 @@
         <f t="shared" si="0"/>
         <v>8.6915123656772231E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>8.6877374334833903E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="d">
         <v>2018-03-07</v>
       </c>
@@ -3200,8 +3298,12 @@
         <f t="shared" si="0"/>
         <v>-3.7339366721997891E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>-3.7409252156789074E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="d">
         <v>2018-03-08</v>
       </c>
@@ -3227,8 +3329,12 @@
         <f t="shared" si="0"/>
         <v>8.7154227285779484E-5</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>8.7150429576768584E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="d">
         <v>2018-03-09</v>
       </c>
@@ -3254,8 +3360,12 @@
         <f t="shared" si="0"/>
         <v>2.8760647778291126E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>2.8354823165339976E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="d">
         <v>2018-03-12</v>
       </c>
@@ -3281,8 +3391,12 @@
         <f t="shared" si="0"/>
         <v>-3.2191945780887243E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>-3.2243873322733894E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="d">
         <v>2018-03-13</v>
       </c>
@@ -3308,8 +3422,12 @@
         <f t="shared" si="0"/>
         <v>-1.198377231544856E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>-1.2056156587219835E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="d">
         <v>2018-03-14</v>
       </c>
@@ -3335,8 +3453,12 @@
         <f t="shared" si="0"/>
         <v>-1.1182793484198594E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>-1.124579101850208E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="d">
         <v>2018-03-15</v>
       </c>
@@ -3362,8 +3484,12 @@
         <f t="shared" si="0"/>
         <v>2.5228075746281942E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>2.5196306376774826E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="d">
         <v>2018-03-16</v>
       </c>
@@ -3389,8 +3515,12 @@
         <f t="shared" si="0"/>
         <v>1.7355874240825298E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>1.7340830326462607E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="d">
         <v>2018-03-19</v>
       </c>
@@ -3416,8 +3546,12 @@
         <f t="shared" si="0"/>
         <v>-7.8829323094162795E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>-7.9141668752445282E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="d">
         <v>2018-03-20</v>
       </c>
@@ -3443,8 +3577,12 @@
         <f t="shared" si="0"/>
         <v>9.6040706665223574E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>9.5994617086017598E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="d">
         <v>2018-03-21</v>
       </c>
@@ -3470,8 +3608,12 @@
         <f t="shared" si="0"/>
         <v>8.7239912565562072E-4</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>8.7201880671559896E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="d">
         <v>2018-03-22</v>
       </c>
@@ -3497,8 +3639,12 @@
         <f t="shared" si="0"/>
         <v>-4.1746593798351772E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>-4.2643020121321901E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="d">
         <v>2018-03-23</v>
       </c>
@@ -3524,8 +3670,12 @@
         <f t="shared" si="0"/>
         <v>-2.6739450389854147E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>-2.7103452981713575E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="d">
         <v>2018-03-26</v>
       </c>
@@ -3551,8 +3701,12 @@
         <f t="shared" si="0"/>
         <v>3.0838210733352689E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>3.0372268116943338E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="d">
         <v>2018-03-27</v>
       </c>
@@ -3578,8 +3732,12 @@
         <f t="shared" si="0"/>
         <v>-1.9399879431309386E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>-1.9590526811013555E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="d">
         <v>2018-03-28</v>
       </c>
@@ -3605,8 +3763,12 @@
         <f t="shared" si="0"/>
         <v>-1.5715331444310365E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>-1.5727692979169263E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="d">
         <v>2018-03-29</v>
       </c>
@@ -3632,8 +3794,12 @@
         <f t="shared" si="0"/>
         <v>1.8240726591535639E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>1.8076360302886729E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="d">
         <v>2018-04-02</v>
       </c>
@@ -3659,8 +3825,12 @@
         <f t="shared" si="0"/>
         <v>-1.9277995351200561E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>-1.9466239139244994E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="d">
         <v>2018-04-03</v>
       </c>
@@ -3686,8 +3856,12 @@
         <f t="shared" si="0"/>
         <v>1.3722772682449147E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>1.362946806702366E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="d">
         <v>2018-04-04</v>
       </c>
@@ -3713,8 +3887,12 @@
         <f t="shared" si="0"/>
         <v>1.5183401486504211E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>1.5069287290785079E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="d">
         <v>2018-04-05</v>
       </c>
@@ -3740,8 +3918,12 @@
         <f t="shared" si="0"/>
         <v>1.3130377956922956E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>1.304492177938809E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="d">
         <v>2018-04-06</v>
       </c>
@@ -3767,8 +3949,12 @@
         <f t="shared" si="0"/>
         <v>-2.4937476078968346E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>-2.5253682941850354E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="d">
         <v>2018-04-09</v>
       </c>
@@ -3794,8 +3980,12 @@
         <f t="shared" si="0"/>
         <v>1.2008537052788482E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48">
+        <f t="shared" si="1"/>
+        <v>1.1937006652605968E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="d">
         <v>2018-04-10</v>
       </c>
@@ -3821,8 +4011,12 @@
         <f t="shared" si="0"/>
         <v>1.9112326291058856E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49">
+        <f t="shared" si="1"/>
+        <v>1.8931980050739251E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="d">
         <v>2018-04-11</v>
       </c>
@@ -3848,8 +4042,12 @@
         <f t="shared" si="0"/>
         <v>-1.6798472080802207E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <f t="shared" si="1"/>
+        <v>-1.6941166704670631E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="d">
         <v>2018-04-12</v>
       </c>
@@ -3875,8 +4073,12 @@
         <f t="shared" si="0"/>
         <v>2.4859902084505281E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <f t="shared" si="1"/>
+        <v>2.4555922355521415E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="d">
         <v>2018-04-13</v>
       </c>
@@ -3902,8 +4104,12 @@
         <f t="shared" si="0"/>
         <v>-2.7079510966139031E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>-2.7452917469336636E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="d">
         <v>2018-04-16</v>
       </c>
@@ -3929,8 +4135,12 @@
         <f t="shared" si="0"/>
         <v>-8.1588815190725139E-4</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <f t="shared" si="1"/>
+        <v>-8.1622116979468287E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="d">
         <v>2018-04-17</v>
       </c>
@@ -3956,8 +4166,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="d">
         <v>2018-04-18</v>
       </c>
@@ -3983,8 +4197,12 @@
         <f t="shared" si="0"/>
         <v>-8.0756111507627182E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>-8.1083955203336295E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="d">
         <v>2018-04-19</v>
       </c>
@@ -4010,8 +4228,12 @@
         <f t="shared" si="0"/>
         <v>2.1953935485667042E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <f t="shared" si="1"/>
+        <v>2.1716417855392325E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="d">
         <v>2018-04-20</v>
       </c>
@@ -4037,8 +4259,12 @@
         <f t="shared" si="0"/>
         <v>-2.2378310657831246E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <f t="shared" si="1"/>
+        <v>-2.2403387516059538E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="d">
         <v>2018-04-23</v>
       </c>
@@ -4064,8 +4290,12 @@
         <f t="shared" si="0"/>
         <v>-4.844189177535263E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <f t="shared" si="1"/>
+        <v>-4.8559602916503648E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="d">
         <v>2018-04-24</v>
       </c>
@@ -4091,8 +4321,12 @@
         <f t="shared" si="0"/>
         <v>-4.6876806625733014E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <f t="shared" si="1"/>
+        <v>-4.6987022949881137E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="d">
         <v>2018-04-25</v>
       </c>
@@ -4118,8 +4352,12 @@
         <f t="shared" si="0"/>
         <v>-3.803994222546625E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <f t="shared" si="1"/>
+        <v>-3.8112478094808233E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="d">
         <v>2018-04-26</v>
       </c>
@@ -4145,8 +4383,12 @@
         <f t="shared" si="0"/>
         <v>1.0000416707571791E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <f t="shared" si="1"/>
+        <v>9.9954196221071763E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="d">
         <v>2018-04-27</v>
       </c>
@@ -4172,8 +4414,12 @@
         <f t="shared" si="0"/>
         <v>-6.35784477931578E-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <f t="shared" si="1"/>
+        <v>-6.3781419510155592E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="d">
         <v>2018-04-30</v>
       </c>
@@ -4199,8 +4445,12 @@
         <f t="shared" si="0"/>
         <v>-5.6672244242629288E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63">
+        <f t="shared" si="1"/>
+        <v>-5.6833440718904778E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="d">
         <v>2018-05-01</v>
       </c>
@@ -4226,8 +4476,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <f>LN(F64/F63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="d">
         <v>2018-05-02</v>
       </c>
@@ -4253,8 +4507,12 @@
         <f t="shared" si="0"/>
         <v>-7.9059993352782465E-3</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65">
+        <f t="shared" si="1"/>
+        <v>-7.9374174519910093E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="d">
         <v>2018-05-03</v>
       </c>
@@ -4280,8 +4538,12 @@
         <f t="shared" si="0"/>
         <v>-6.3008653158677097E-3</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66">
+        <f t="shared" si="1"/>
+        <v>-6.3207995471183283E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="d">
         <v>2018-05-04</v>
       </c>
@@ -4307,8 +4569,12 @@
         <f t="shared" si="0"/>
         <v>1.1096581131067706E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67">
+        <f t="shared" si="1"/>
+        <v>1.1035465773398043E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="d">
         <v>2018-05-07</v>
       </c>
@@ -4331,11 +4597,15 @@
         <v>9356700</v>
       </c>
       <c r="K68">
-        <f t="shared" ref="K68:K131" si="1">(F68/F67)-1</f>
+        <f t="shared" ref="K68:K131" si="2">(F68/F67)-1</f>
         <v>8.6692195306630193E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68">
+        <f t="shared" ref="L68:L131" si="3">LN(F68/F67)</f>
+        <v>8.6318576241276486E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="d">
         <v>2018-05-08</v>
       </c>
@@ -4358,11 +4628,15 @@
         <v>12543200</v>
       </c>
       <c r="K69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4812115229976497E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69">
+        <f t="shared" si="3"/>
+        <v>1.4703487211316518E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="d">
         <v>2018-05-09</v>
       </c>
@@ -4385,11 +4659,15 @@
         <v>11368100</v>
       </c>
       <c r="K70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.180373776601896E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70">
+        <f t="shared" si="3"/>
+        <v>2.1569435929027724E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="d">
         <v>2018-05-10</v>
       </c>
@@ -4412,11 +4690,15 @@
         <v>9159700</v>
       </c>
       <c r="K71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.7595225239694976E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71">
+        <f t="shared" si="3"/>
+        <v>7.7295722624506676E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="d">
         <v>2018-05-11</v>
       </c>
@@ -4439,11 +4721,15 @@
         <v>10253000</v>
       </c>
       <c r="K72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.7624544703477314E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72">
+        <f t="shared" si="3"/>
+        <v>-3.769550306266565E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="d">
         <v>2018-05-14</v>
       </c>
@@ -4466,11 +4752,15 @@
         <v>8710700</v>
       </c>
       <c r="K73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5140051225446278E-4</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L73">
+        <f t="shared" si="3"/>
+        <v>3.5133878555456235E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="d">
         <v>2018-05-15</v>
       </c>
@@ -4493,11 +4783,15 @@
         <v>11536200</v>
       </c>
       <c r="K74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.638457575363522E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L74">
+        <f t="shared" si="3"/>
+        <v>-7.6677800066298745E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="d">
         <v>2018-05-16</v>
       </c>
@@ -4520,11 +4814,15 @@
         <v>7571100</v>
       </c>
       <c r="K75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7426833377381943E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L75">
+        <f t="shared" si="3"/>
+        <v>2.7389290447838101E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="d">
         <v>2018-05-17</v>
       </c>
@@ -4547,11 +4845,15 @@
         <v>8617200</v>
       </c>
       <c r="K76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.3527162867190707E-3</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L76">
+        <f t="shared" si="3"/>
+        <v>-3.3583492339419379E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="d">
         <v>2018-05-18</v>
       </c>
@@ -4574,11 +4876,15 @@
         <v>11806300</v>
       </c>
       <c r="K77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6200435321194417E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L77">
+        <f t="shared" si="3"/>
+        <v>-1.6333097110520233E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="d">
         <v>2018-05-21</v>
       </c>
@@ -4601,11 +4907,15 @@
         <v>9441900</v>
       </c>
       <c r="K78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1785104351025382E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L78">
+        <f t="shared" si="3"/>
+        <v>9.1366438948563052E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="d">
         <v>2018-05-22</v>
       </c>
@@ -4628,11 +4938,15 @@
         <v>11507600</v>
       </c>
       <c r="K79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.6682286778455566E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L79">
+        <f t="shared" si="3"/>
+        <v>7.6389772548827286E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="d">
         <v>2018-05-23</v>
       </c>
@@ -4655,11 +4969,15 @@
         <v>11453900</v>
       </c>
       <c r="K80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.601329008859345E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L80">
+        <f t="shared" si="3"/>
+        <v>-4.6119477091264424E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="d">
         <v>2018-05-24</v>
       </c>
@@ -4682,11 +5000,15 @@
         <v>14084800</v>
       </c>
       <c r="K81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.120097874106607E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L81">
+        <f t="shared" si="3"/>
+        <v>-1.1264182106330531E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="d">
         <v>2018-05-25</v>
       </c>
@@ -4709,11 +5031,15 @@
         <v>8283500</v>
       </c>
       <c r="K82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.1244042955550517E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L82">
+        <f t="shared" si="3"/>
+        <v>-5.1375790831455206E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="d">
         <v>2018-05-29</v>
       </c>
@@ -4736,11 +5062,15 @@
         <v>30643800</v>
       </c>
       <c r="K83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.2743602269087355E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L83">
+        <f t="shared" si="3"/>
+        <v>-4.3684005198738607E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="d">
         <v>2018-05-30</v>
       </c>
@@ -4763,11 +5093,15 @@
         <v>17490800</v>
       </c>
       <c r="K84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2845245146959625E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L84">
+        <f t="shared" si="3"/>
+        <v>2.2588200010025958E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="d">
         <v>2018-05-31</v>
       </c>
@@ -4790,11 +5124,15 @@
         <v>19808200</v>
       </c>
       <c r="K85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.2367340728118514E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L85">
+        <f t="shared" si="3"/>
+        <v>-1.2444452726297664E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="d">
         <v>2018-06-01</v>
       </c>
@@ -4817,11 +5155,15 @@
         <v>13594200</v>
       </c>
       <c r="K86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2989439868372976E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L86">
+        <f t="shared" si="3"/>
+        <v>1.290580060053444E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="d">
         <v>2018-06-04</v>
       </c>
@@ -4844,11 +5186,15 @@
         <v>9415400</v>
       </c>
       <c r="K87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6125102492000636E-4</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L87">
+        <f t="shared" si="3"/>
+        <v>4.6114468136547053E-4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="d">
         <v>2018-06-05</v>
       </c>
@@ -4871,11 +5217,15 @@
         <v>10415200</v>
       </c>
       <c r="K88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.6247693590414372E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L88">
+        <f t="shared" si="3"/>
+        <v>-5.6406479444597772E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="d">
         <v>2018-06-06</v>
       </c>
@@ -4898,11 +5248,15 @@
         <v>15453600</v>
       </c>
       <c r="K89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3367975825464793E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L89">
+        <f t="shared" si="3"/>
+        <v>2.3099124956183888E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="d">
         <v>2018-06-07</v>
       </c>
@@ -4925,11 +5279,15 @@
         <v>13444400</v>
       </c>
       <c r="K90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9869622342327826E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L90">
+        <f t="shared" si="3"/>
+        <v>3.9790353627436222E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="d">
         <v>2018-06-08</v>
       </c>
@@ -4952,11 +5310,15 @@
         <v>10383200</v>
       </c>
       <c r="K91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7978739512133366E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L91">
+        <f t="shared" si="3"/>
+        <v>2.7939671872820896E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="d">
         <v>2018-06-11</v>
       </c>
@@ -4979,11 +5341,15 @@
         <v>12642900</v>
       </c>
       <c r="K92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.5200876055135879E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L92">
+        <f t="shared" si="3"/>
+        <v>-2.5232683712793375E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="d">
         <v>2018-06-12</v>
       </c>
@@ -5006,11 +5372,15 @@
         <v>15294100</v>
       </c>
       <c r="K93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.7744941142447992E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L93">
+        <f t="shared" si="3"/>
+        <v>-5.7912309677244584E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="d">
         <v>2018-06-13</v>
       </c>
@@ -5033,11 +5403,15 @@
         <v>14979700</v>
       </c>
       <c r="K94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.996594031651755E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L94">
+        <f t="shared" si="3"/>
+        <v>-1.998589882560528E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="d">
         <v>2018-06-14</v>
       </c>
@@ -5060,11 +5434,15 @@
         <v>20487300</v>
       </c>
       <c r="K95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.7641191721618044E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L95">
+        <f t="shared" si="3"/>
+        <v>-1.7798652152390265E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="d">
         <v>2018-06-15</v>
       </c>
@@ -5087,11 +5465,15 @@
         <v>26028600</v>
       </c>
       <c r="K96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.2034060902538224E-3</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L96">
+        <f t="shared" si="3"/>
+        <v>-1.2041307648063733E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="d">
         <v>2018-06-18</v>
       </c>
@@ -5114,11 +5496,15 @@
         <v>9786800</v>
       </c>
       <c r="K97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5949253455705978E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L97">
+        <f t="shared" si="3"/>
+        <v>2.5915643399129825E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="d">
         <v>2018-06-19</v>
       </c>
@@ -5141,11 +5527,15 @@
         <v>12707200</v>
       </c>
       <c r="K98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.8234753435302267E-3</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L98">
+        <f t="shared" si="3"/>
+        <v>-5.8404978951797464E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="d">
         <v>2018-06-20</v>
       </c>
@@ -5168,11 +5558,15 @@
         <v>8876900</v>
       </c>
       <c r="K99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.3023582812046257E-5</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L99">
+        <f t="shared" si="3"/>
+        <v>-9.3027909773867599E-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="d">
         <v>2018-06-21</v>
       </c>
@@ -5195,11 +5589,15 @@
         <v>11048700</v>
       </c>
       <c r="K100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.7894260439753626E-4</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L100">
+        <f t="shared" si="3"/>
+        <v>-2.7898151612207041E-4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="d">
         <v>2018-06-22</v>
       </c>
@@ -5222,11 +5620,15 @@
         <v>19478900</v>
       </c>
       <c r="K101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6370650433813139E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L101">
+        <f t="shared" si="3"/>
+        <v>-1.6506130160721933E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="d">
         <v>2018-06-25</v>
       </c>
@@ -5249,11 +5651,15 @@
         <v>16907600</v>
       </c>
       <c r="K102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.0779792902703216E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L102">
+        <f t="shared" si="3"/>
+        <v>-9.1194352257394761E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="d">
         <v>2018-06-26</v>
       </c>
@@ -5276,11 +5682,15 @@
         <v>17086800</v>
       </c>
       <c r="K103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.6799946303852664E-4</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L103">
+        <f t="shared" si="3"/>
+        <v>6.6777645070643563E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="d">
         <v>2018-06-27</v>
       </c>
@@ -5303,11 +5713,15 @@
         <v>16276800</v>
       </c>
       <c r="K104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.5449180823768227E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L104">
+        <f t="shared" si="3"/>
+        <v>-1.5569762960191568E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="d">
         <v>2018-06-28</v>
       </c>
@@ -5330,11 +5744,15 @@
         <v>14491300</v>
       </c>
       <c r="K105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.636963176251971E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L105">
+        <f t="shared" si="3"/>
+        <v>1.6237093783073083E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="d">
         <v>2018-06-29</v>
       </c>
@@ -5357,11 +5775,15 @@
         <v>18972400</v>
       </c>
       <c r="K106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.9571308374991592E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L106">
+        <f t="shared" si="3"/>
+        <v>-6.9814445067858041E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="d">
         <v>2018-07-02</v>
       </c>
@@ -5384,11 +5806,15 @@
         <v>11130000</v>
       </c>
       <c r="K107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4454496481831676E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L107">
+        <f t="shared" si="3"/>
+        <v>8.4099863673102026E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="d">
         <v>2018-07-03</v>
       </c>
@@ -5411,11 +5837,15 @@
         <v>8311700</v>
       </c>
       <c r="K108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.3989303378223794E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L108">
+        <f t="shared" si="3"/>
+        <v>-1.4088075937558966E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="d">
         <v>2018-07-05</v>
       </c>
@@ -5438,11 +5868,15 @@
         <v>10723400</v>
       </c>
       <c r="K109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5016480752146943E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L109">
+        <f t="shared" si="3"/>
+        <v>6.4806035282758299E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="d">
         <v>2018-07-06</v>
       </c>
@@ -5465,11 +5899,15 @@
         <v>12173700</v>
       </c>
       <c r="K110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2780169626294153E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L110">
+        <f t="shared" si="3"/>
+        <v>3.2726559774313045E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="d">
         <v>2018-07-09</v>
       </c>
@@ -5492,11 +5930,15 @@
         <v>13900800</v>
       </c>
       <c r="K111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0943601518156338E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L111">
+        <f t="shared" si="3"/>
+        <v>3.0474500840376235E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="d">
         <v>2018-07-10</v>
       </c>
@@ -5519,11 +5961,15 @@
         <v>14575900</v>
       </c>
       <c r="K112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.1520295951333903E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L112">
+        <f t="shared" si="3"/>
+        <v>-6.1710313019970528E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="d">
         <v>2018-07-11</v>
       </c>
@@ -5546,11 +5992,15 @@
         <v>10186500</v>
       </c>
       <c r="K113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.1571878291933855E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L113">
+        <f t="shared" si="3"/>
+        <v>-2.1595179104102365E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="d">
         <v>2018-07-12</v>
       </c>
@@ -5573,11 +6023,15 @@
         <v>12456800</v>
       </c>
       <c r="K114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3237026972222647E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L114">
+        <f t="shared" si="3"/>
+        <v>4.3143823506626728E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="d">
         <v>2018-07-13</v>
       </c>
@@ -5600,11 +6054,15 @@
         <v>21289100</v>
       </c>
       <c r="K115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.585790457301564E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L115">
+        <f t="shared" si="3"/>
+        <v>-4.5963374509148018E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="d">
         <v>2018-07-16</v>
       </c>
@@ -5627,11 +6085,15 @@
         <v>24662600</v>
       </c>
       <c r="K116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.967649376855209E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L116">
+        <f t="shared" si="3"/>
+        <v>3.8909601078853745E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="d">
         <v>2018-07-17</v>
       </c>
@@ -5654,11 +6116,15 @@
         <v>14821900</v>
       </c>
       <c r="K117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-7.2342535364944283E-4</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L117">
+        <f t="shared" si="3"/>
+        <v>-7.236871520392707E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="d">
         <v>2018-07-18</v>
       </c>
@@ -5681,11 +6147,15 @@
         <v>14244900</v>
       </c>
       <c r="K118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.3212126216026814E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L118">
+        <f t="shared" si="3"/>
+        <v>9.2780382038154269E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="d">
         <v>2018-07-19</v>
       </c>
@@ -5708,11 +6178,15 @@
         <v>16775300</v>
       </c>
       <c r="K119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.4704590681948626E-2</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L119">
+        <f t="shared" si="3"/>
+        <v>-1.4813774836335851E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="d">
         <v>2018-07-20</v>
       </c>
@@ -5735,11 +6209,15 @@
         <v>13578100</v>
       </c>
       <c r="K120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2649026119504914E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L120">
+        <f t="shared" si="3"/>
+        <v>1.2569695458586848E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="d">
         <v>2018-07-23</v>
       </c>
@@ -5762,11 +6240,15 @@
         <v>18140000</v>
       </c>
       <c r="K121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8601739611639134E-2</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L121">
+        <f t="shared" si="3"/>
+        <v>1.8430843312617771E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="d">
         <v>2018-07-24</v>
       </c>
@@ -5789,11 +6271,15 @@
         <v>14000400</v>
       </c>
       <c r="K122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0578840907637996E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L122">
+        <f t="shared" si="3"/>
+        <v>7.0330938031472256E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="d">
         <v>2018-07-25</v>
       </c>
@@ -5816,11 +6302,15 @@
         <v>13329100</v>
       </c>
       <c r="K123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0232342616864969E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L123">
+        <f t="shared" si="3"/>
+        <v>8.9827681248740021E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="d">
         <v>2018-07-26</v>
       </c>
@@ -5843,11 +6333,15 @@
         <v>11897800</v>
       </c>
       <c r="K124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.8651429665071948E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L124">
+        <f t="shared" si="3"/>
+        <v>-2.8692553455307019E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="d">
         <v>2018-07-27</v>
       </c>
@@ -5870,11 +6364,15 @@
         <v>12802700</v>
       </c>
       <c r="K125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0274244494558715E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L125">
+        <f t="shared" si="3"/>
+        <v>1.0221823198319303E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="d">
         <v>2018-07-30</v>
       </c>
@@ -5897,11 +6395,15 @@
         <v>13411600</v>
       </c>
       <c r="K126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0329599078920992E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L126">
+        <f t="shared" si="3"/>
+        <v>6.0148344687659099E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="d">
         <v>2018-07-31</v>
       </c>
@@ -5924,11 +6426,15 @@
         <v>15843800</v>
       </c>
       <c r="K127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.5248879408313765E-2</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L127">
+        <f t="shared" si="3"/>
+        <v>-1.5366339186416385E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="d">
         <v>2018-08-01</v>
       </c>
@@ -5951,11 +6457,15 @@
         <v>13531600</v>
       </c>
       <c r="K128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.1766097745648008E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L128">
+        <f t="shared" si="3"/>
+        <v>6.1576127052687842E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="d">
         <v>2018-08-02</v>
       </c>
@@ -5978,11 +6488,15 @@
         <v>11058100</v>
       </c>
       <c r="K129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2365459056152854E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L129">
+        <f t="shared" si="3"/>
+        <v>4.2275970110421069E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="d">
         <v>2018-08-03</v>
       </c>
@@ -6005,11 +6519,15 @@
         <v>11016100</v>
       </c>
       <c r="K130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0929178673474489E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L130">
+        <f t="shared" si="3"/>
+        <v>8.0603458247784712E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="d">
         <v>2018-08-06</v>
       </c>
@@ -6032,11 +6550,15 @@
         <v>9857400</v>
       </c>
       <c r="K131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5628515386544315E-4</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L131">
+        <f t="shared" si="3"/>
+        <v>2.5625231843543291E-4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="d">
         <v>2018-08-07</v>
       </c>
@@ -6059,11 +6581,15 @@
         <v>10562100</v>
       </c>
       <c r="K132">
-        <f t="shared" ref="K132:K195" si="2">(F132/F131)-1</f>
+        <f t="shared" ref="K132:K195" si="4">(F132/F131)-1</f>
         <v>3.6714971137197239E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L132">
+        <f t="shared" ref="L132:L195" si="5">LN(F132/F131)</f>
+        <v>3.6647736200248878E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="d">
         <v>2018-08-08</v>
       </c>
@@ -6086,11 +6612,15 @@
         <v>8997100</v>
       </c>
       <c r="K133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.0416618235434836E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L133">
+        <f t="shared" si="5"/>
+        <v>2.0395804645153351E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="d">
         <v>2018-08-09</v>
       </c>
@@ -6113,11 +6643,15 @@
         <v>9694200</v>
       </c>
       <c r="K134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-7.7257482725500148E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L134">
+        <f t="shared" si="5"/>
+        <v>-7.7557464713081713E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="d">
         <v>2018-08-10</v>
       </c>
@@ -6140,11 +6674,15 @@
         <v>12630600</v>
       </c>
       <c r="K135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-9.8390543595265889E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L135">
+        <f t="shared" si="5"/>
+        <v>-9.8877777127784183E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="d">
         <v>2018-08-13</v>
       </c>
@@ -6167,11 +6705,15 @@
         <v>10336300</v>
       </c>
       <c r="K136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.5899164753229611E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L136">
+        <f t="shared" si="5"/>
+        <v>-1.602691233579296E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="d">
         <v>2018-08-14</v>
       </c>
@@ -6194,11 +6736,15 @@
         <v>10597600</v>
       </c>
       <c r="K137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.6732198226848727E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L137">
+        <f t="shared" si="5"/>
+        <v>6.6510524551141783E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="d">
         <v>2018-08-15</v>
       </c>
@@ -6221,11 +6767,15 @@
         <v>10152100</v>
       </c>
       <c r="K138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-8.2860761970946495E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L138">
+        <f t="shared" si="5"/>
+        <v>-8.3205965509139425E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="d">
         <v>2018-08-16</v>
       </c>
@@ -6248,11 +6798,15 @@
         <v>10118600</v>
       </c>
       <c r="K139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.4106700143063993E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L139">
+        <f t="shared" si="5"/>
+        <v>9.3666655183505948E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="d">
         <v>2018-08-17</v>
       </c>
@@ -6275,11 +6829,15 @@
         <v>8505100</v>
       </c>
       <c r="K140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L140">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="d">
         <v>2018-08-20</v>
       </c>
@@ -6302,11 +6860,15 @@
         <v>8618700</v>
       </c>
       <c r="K141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.3069249753614454E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L141">
+        <f t="shared" si="5"/>
+        <v>-1.3077797466361759E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="d">
         <v>2018-08-21</v>
       </c>
@@ -6329,11 +6891,15 @@
         <v>10976700</v>
       </c>
       <c r="K142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.1070304739807568E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L142">
+        <f t="shared" si="5"/>
+        <v>6.0884581395603647E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="d">
         <v>2018-08-22</v>
       </c>
@@ -6356,11 +6922,15 @@
         <v>8314700</v>
       </c>
       <c r="K143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3.0349090518883015E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L143">
+        <f t="shared" si="5"/>
+        <v>-3.0395237274772405E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="d">
         <v>2018-08-23</v>
       </c>
@@ -6383,11 +6953,15 @@
         <v>9265400</v>
       </c>
       <c r="K144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.08747807686116E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L144">
+        <f t="shared" si="5"/>
+        <v>-2.0896598960838232E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="d">
         <v>2018-08-24</v>
       </c>
@@ -6410,11 +6984,15 @@
         <v>8845700</v>
       </c>
       <c r="K145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.3590724562592165E-4</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L145">
+        <f t="shared" si="5"/>
+        <v>-4.3600228080800267E-4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="d">
         <v>2018-08-27</v>
       </c>
@@ -6437,11 +7015,15 @@
         <v>13768000</v>
       </c>
       <c r="K146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7701468398308329E-2</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L146">
+        <f t="shared" si="5"/>
+        <v>1.7546622074399679E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="d">
         <v>2018-08-28</v>
       </c>
@@ -6464,11 +7046,15 @@
         <v>8302600</v>
       </c>
       <c r="K147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.8839304856110877E-3</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L147">
+        <f t="shared" si="5"/>
+        <v>-4.8958958486702226E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="d">
         <v>2018-08-29</v>
       </c>
@@ -6491,11 +7077,15 @@
         <v>7221700</v>
       </c>
       <c r="K148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3.271871461352438E-3</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L148">
+        <f t="shared" si="5"/>
+        <v>-3.2772357367912655E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="d">
         <v>2018-08-30</v>
       </c>
@@ -6518,11 +7108,15 @@
         <v>8991800</v>
       </c>
       <c r="K149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.9239398659780553E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L149">
+        <f t="shared" si="5"/>
+        <v>-4.9361023993608096E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="d">
         <v>2018-08-31</v>
       </c>
@@ -6545,11 +7139,15 @@
         <v>13065700</v>
       </c>
       <c r="K150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.2956131788822747E-3</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L150">
+        <f t="shared" si="5"/>
+        <v>-5.3096846383416446E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="d">
         <v>2018-09-04</v>
       </c>
@@ -6572,11 +7170,15 @@
         <v>10174200</v>
       </c>
       <c r="K151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9747207664316839E-3</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L151">
+        <f t="shared" si="5"/>
+        <v>4.9623877284482067E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="d">
         <v>2018-09-05</v>
       </c>
@@ -6599,11 +7201,15 @@
         <v>11462400</v>
       </c>
       <c r="K152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.8633411096702384E-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L152">
+        <f t="shared" si="5"/>
+        <v>-4.8752056361683286E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="d">
         <v>2018-09-06</v>
       </c>
@@ -6626,11 +7232,15 @@
         <v>9877600</v>
       </c>
       <c r="K153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.2761055629234601E-3</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L153">
+        <f t="shared" si="5"/>
+        <v>-4.2852742491647838E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="d">
         <v>2018-09-07</v>
       </c>
@@ -6653,11 +7263,15 @@
         <v>10955600</v>
       </c>
       <c r="K154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9281452285551115E-3</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L154">
+        <f t="shared" si="5"/>
+        <v>1.9262887425439605E-3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="d">
         <v>2018-09-10</v>
       </c>
@@ -6680,11 +7294,15 @@
         <v>8276900</v>
       </c>
       <c r="K155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.3358422937195282E-3</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L155">
+        <f t="shared" si="5"/>
+        <v>-5.350128743033462E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="d">
         <v>2018-09-11</v>
       </c>
@@ -6707,11 +7325,15 @@
         <v>9333800</v>
       </c>
       <c r="K156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3318815806649997E-3</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L156">
+        <f t="shared" si="5"/>
+        <v>6.3119194394517849E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="d">
         <v>2018-09-12</v>
       </c>
@@ -6734,11 +7356,15 @@
         <v>10800800</v>
       </c>
       <c r="K157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.1797633370114302E-2</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L157">
+        <f t="shared" si="5"/>
+        <v>-1.1867777683772382E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="d">
         <v>2018-09-13</v>
       </c>
@@ -6761,11 +7387,15 @@
         <v>12470800</v>
       </c>
       <c r="K158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.891083834417941E-3</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L158">
+        <f t="shared" si="5"/>
+        <v>3.8835331482785147E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="d">
         <v>2018-09-14</v>
       </c>
@@ -6788,11 +7418,15 @@
         <v>10337900</v>
       </c>
       <c r="K159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.7620872085888362E-4</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L159">
+        <f t="shared" si="5"/>
+        <v>-1.7622424743950972E-4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="d">
         <v>2018-09-17</v>
       </c>
@@ -6815,11 +7449,15 @@
         <v>9561300</v>
       </c>
       <c r="K160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9956314373820181E-3</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L160">
+        <f t="shared" si="5"/>
+        <v>2.9911534741836848E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="d">
         <v>2018-09-18</v>
       </c>
@@ -6842,11 +7480,15 @@
         <v>7944200</v>
       </c>
       <c r="K161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.0406752683190827E-3</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L161">
+        <f t="shared" si="5"/>
+        <v>4.0325336643565581E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="d">
         <v>2018-09-19</v>
       </c>
@@ -6869,11 +7511,15 @@
         <v>16052800</v>
       </c>
       <c r="K162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.9046496550343415E-2</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L162">
+        <f t="shared" si="5"/>
+        <v>2.863264198298638E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="d">
         <v>2018-09-20</v>
       </c>
@@ -6896,11 +7542,15 @@
         <v>15590000</v>
       </c>
       <c r="K163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.5868261275527935E-3</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L163">
+        <f t="shared" si="5"/>
+        <v>8.5501690320092805E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="d">
         <v>2018-09-21</v>
       </c>
@@ -6923,11 +7573,15 @@
         <v>24788200</v>
       </c>
       <c r="K164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-6.5749936612824467E-3</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L164">
+        <f t="shared" si="5"/>
+        <v>-6.5967041486422132E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="d">
         <v>2018-09-24</v>
       </c>
@@ -6950,11 +7604,15 @@
         <v>12492500</v>
       </c>
       <c r="K165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-9.5884756258607373E-3</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L165">
+        <f t="shared" si="5"/>
+        <v>-9.6347410389918762E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="d">
         <v>2018-09-25</v>
       </c>
@@ -6977,11 +7635,15 @@
         <v>9308300</v>
       </c>
       <c r="K166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.8271994379494014E-3</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L166">
+        <f t="shared" si="5"/>
+        <v>-2.8312035149439222E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="d">
         <v>2018-09-26</v>
       </c>
@@ -7004,11 +7666,15 @@
         <v>14023600</v>
       </c>
       <c r="K167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.177082518285677E-2</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L167">
+        <f t="shared" si="5"/>
+        <v>-1.1840649815493626E-2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="d">
         <v>2018-09-27</v>
       </c>
@@ -7031,11 +7697,15 @@
         <v>13283000</v>
       </c>
       <c r="K168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-4.3471059355245645E-3</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L168">
+        <f t="shared" si="5"/>
+        <v>-4.3565820730192689E-3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="d">
         <v>2018-09-28</v>
       </c>
@@ -7058,11 +7728,15 @@
         <v>15815100</v>
       </c>
       <c r="K169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.4669946005479217E-2</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L169">
+        <f t="shared" si="5"/>
+        <v>-1.4778613739396871E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="d">
         <v>2018-10-01</v>
       </c>
@@ -7085,11 +7759,15 @@
         <v>10146300</v>
       </c>
       <c r="K170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.8490353747302493E-3</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L170">
+        <f t="shared" si="5"/>
+        <v>5.8319961769520865E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="d">
         <v>2018-10-02</v>
       </c>
@@ -7112,11 +7790,15 @@
         <v>13753100</v>
       </c>
       <c r="K171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.140940374671942E-3</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L171">
+        <f t="shared" si="5"/>
+        <v>4.1323902765824103E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="d">
         <v>2018-10-03</v>
       </c>
@@ -7139,11 +7821,15 @@
         <v>17142000</v>
       </c>
       <c r="K172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.3885030632290256E-3</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L172">
+        <f t="shared" si="5"/>
+        <v>9.3447049871854555E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="d">
         <v>2018-10-04</v>
       </c>
@@ -7166,11 +7852,15 @@
         <v>16357400</v>
       </c>
       <c r="K173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.0160138065620288E-3</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L173">
+        <f t="shared" si="5"/>
+        <v>8.9756122133807931E-3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="d">
         <v>2018-10-05</v>
       </c>
@@ -7193,11 +7883,15 @@
         <v>13777600</v>
       </c>
       <c r="K174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.638859419291653E-3</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L174">
+        <f t="shared" si="5"/>
+        <v>-5.6548178067445361E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="d">
         <v>2018-10-08</v>
       </c>
@@ -7220,11 +7914,15 @@
         <v>14370900</v>
       </c>
       <c r="K175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.1070464200378982E-3</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L175">
+        <f t="shared" si="5"/>
+        <v>6.0884739888254344E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="d">
         <v>2018-10-09</v>
       </c>
@@ -7247,11 +7945,15 @@
         <v>14069500</v>
       </c>
       <c r="K176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-6.9371898356732631E-3</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L176">
+        <f t="shared" si="5"/>
+        <v>-6.9613640024761593E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="d">
         <v>2018-10-10</v>
       </c>
@@ -7274,11 +7976,15 @@
         <v>23086400</v>
       </c>
       <c r="K177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.6632874504513904E-2</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L177">
+        <f t="shared" si="5"/>
+        <v>-2.6993955015759769E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="d">
         <v>2018-10-11</v>
       </c>
@@ -7301,11 +8007,15 @@
         <v>33705600</v>
       </c>
       <c r="K178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-2.9963239226650562E-2</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L178">
+        <f t="shared" si="5"/>
+        <v>-3.0421310498324448E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="d">
         <v>2018-10-12</v>
       </c>
@@ -7328,11 +8038,15 @@
         <v>32075700</v>
       </c>
       <c r="K179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.0912809045407257E-2</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L179">
+        <f t="shared" si="5"/>
+        <v>-1.0972790522812357E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="d">
         <v>2018-10-15</v>
       </c>
@@ -7355,11 +8069,15 @@
         <v>18903200</v>
       </c>
       <c r="K180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.703649351298079E-3</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L180">
+        <f t="shared" si="5"/>
+        <v>-5.7199772746922275E-3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="d">
         <v>2018-10-16</v>
       </c>
@@ -7382,11 +8100,15 @@
         <v>19302800</v>
       </c>
       <c r="K181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.1440762734332042E-2</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L181">
+        <f t="shared" si="5"/>
+        <v>2.1214143123476241E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="d">
         <v>2018-10-17</v>
       </c>
@@ -7409,11 +8131,15 @@
         <v>18794500</v>
       </c>
       <c r="K182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1139802386684883E-2</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L182">
+        <f t="shared" si="5"/>
+        <v>1.1078211770825479E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="d">
         <v>2018-10-18</v>
       </c>
@@ -7436,11 +8162,15 @@
         <v>17582500</v>
       </c>
       <c r="K183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.5842746108779671E-2</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L183">
+        <f t="shared" si="5"/>
+        <v>-1.5969583833218282E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="d">
         <v>2018-10-19</v>
       </c>
@@ -7463,11 +8193,15 @@
         <v>15234500</v>
       </c>
       <c r="K184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.6652839068708181E-3</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L184">
+        <f t="shared" si="5"/>
+        <v>-1.6666720334133061E-3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="d">
         <v>2018-10-22</v>
       </c>
@@ -7490,11 +8224,15 @@
         <v>16199100</v>
       </c>
       <c r="K185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.4363775656134115E-2</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L185">
+        <f t="shared" si="5"/>
+        <v>-1.4467933282635423E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="d">
         <v>2018-10-23</v>
       </c>
@@ -7517,11 +8255,15 @@
         <v>21407500</v>
       </c>
       <c r="K186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.043623846922348E-2</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L186">
+        <f t="shared" si="5"/>
+        <v>-1.0491077884410191E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="d">
         <v>2018-10-24</v>
       </c>
@@ -7544,11 +8286,15 @@
         <v>23168900</v>
       </c>
       <c r="K187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.8622352084892935E-2</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L187">
+        <f t="shared" si="5"/>
+        <v>-1.8797931298862192E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="d">
         <v>2018-10-25</v>
       </c>
@@ -7571,11 +8317,15 @@
         <v>17464700</v>
       </c>
       <c r="K188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5199984493652119E-2</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L188">
+        <f t="shared" si="5"/>
+        <v>1.5085622143860396E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="d">
         <v>2018-10-26</v>
       </c>
@@ -7598,11 +8348,15 @@
         <v>19174900</v>
       </c>
       <c r="K189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.3732713607721103E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L189">
+        <f t="shared" si="5"/>
+        <v>-1.3827879581710379E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="d">
         <v>2018-10-29</v>
       </c>
@@ -7625,11 +8379,15 @@
         <v>18445200</v>
       </c>
       <c r="K190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3827173619607169E-2</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L190">
+        <f t="shared" si="5"/>
+        <v>1.3732450425057011E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="d">
         <v>2018-10-30</v>
       </c>
@@ -7652,11 +8410,15 @@
         <v>18019700</v>
       </c>
       <c r="K191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.7644230426795859E-2</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L191">
+        <f t="shared" si="5"/>
+        <v>1.7490378094263431E-2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="d">
         <v>2018-10-31</v>
       </c>
@@ -7679,11 +8441,15 @@
         <v>20860000</v>
       </c>
       <c r="K192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.1743096273615814E-2</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L192">
+        <f t="shared" si="5"/>
+        <v>2.1510086672714306E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="d">
         <v>2018-11-01</v>
       </c>
@@ -7706,11 +8472,15 @@
         <v>13065000</v>
       </c>
       <c r="K193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-3.6676761307508077E-4</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L193">
+        <f t="shared" si="5"/>
+        <v>-3.6683488876628048E-4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="d">
         <v>2018-11-02</v>
       </c>
@@ -7733,11 +8503,15 @@
         <v>19009200</v>
       </c>
       <c r="K194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.5056636282296845E-3</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L194">
+        <f t="shared" si="5"/>
+        <v>-5.5208756547836533E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="d">
         <v>2018-11-05</v>
       </c>
@@ -7760,11 +8534,15 @@
         <v>10276400</v>
       </c>
       <c r="K195">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.5509867333208849E-3</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L195">
+        <f t="shared" si="5"/>
+        <v>6.5296222744953116E-3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="d">
         <v>2018-11-06</v>
       </c>
@@ -7787,11 +8565,15 @@
         <v>10825000</v>
       </c>
       <c r="K196">
-        <f t="shared" ref="K196:K204" si="3">(F196/F195)-1</f>
+        <f t="shared" ref="K196:K204" si="6">(F196/F195)-1</f>
         <v>4.6751079087465897E-3</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L196">
+        <f t="shared" ref="L196:L232" si="7">LN(F196/F195)</f>
+        <v>4.6642135334916289E-3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="d">
         <v>2018-11-07</v>
       </c>
@@ -7814,11 +8596,15 @@
         <v>12679600</v>
       </c>
       <c r="K197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.7153358581932565E-2</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L197">
+        <f t="shared" si="7"/>
+        <v>1.7007900763803548E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="d">
         <v>2018-11-08</v>
       </c>
@@ -7841,11 +8627,15 @@
         <v>11662500</v>
       </c>
       <c r="K198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8.0731562091278519E-3</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L198">
+        <f t="shared" si="7"/>
+        <v>8.0407426199886247E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="d">
         <v>2018-11-09</v>
       </c>
@@ -7868,11 +8658,15 @@
         <v>10432200</v>
       </c>
       <c r="K199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-9.6993184428051382E-3</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L199">
+        <f t="shared" si="7"/>
+        <v>-9.7466632220613632E-3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="d">
         <v>2018-11-12</v>
       </c>
@@ -7895,11 +8689,15 @@
         <v>13279700</v>
       </c>
       <c r="K200">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.1026082936946855E-2</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L200">
+        <f t="shared" si="7"/>
+        <v>-2.1250279234475915E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="d">
         <v>2018-11-13</v>
       </c>
@@ -7922,11 +8720,15 @@
         <v>13746100</v>
       </c>
       <c r="K201">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.8741829776911558E-3</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L201">
+        <f t="shared" si="7"/>
+        <v>5.8569972334918743E-3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="d">
         <v>2018-11-14</v>
       </c>
@@ -7949,11 +8751,15 @@
         <v>18361400</v>
       </c>
       <c r="K202">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.0622237978106917E-2</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L202">
+        <f t="shared" si="7"/>
+        <v>-2.0837845687552221E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="d">
         <v>2018-11-15</v>
       </c>
@@ -7976,11 +8782,15 @@
         <v>19100000</v>
       </c>
       <c r="K203">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.5528772953441692E-2</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L203">
+        <f t="shared" si="7"/>
+        <v>2.5208355624204492E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="d">
         <v>2018-11-16</v>
       </c>
@@ -8003,11 +8813,15 @@
         <v>13798600</v>
       </c>
       <c r="K204">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-7.2683505566684126E-4</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L204">
+        <f t="shared" si="7"/>
+        <v>-7.2709932832876363E-4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="d">
         <v>2018-11-19</v>
       </c>
@@ -8033,8 +8847,12 @@
         <f>(F205/F204)-1</f>
         <v>7.6370401231382612E-3</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L205">
+        <f t="shared" si="7"/>
+        <v>7.6080255621614155E-3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="d">
         <v>2018-11-20</v>
       </c>
@@ -8057,11 +8875,15 @@
         <v>18936200</v>
       </c>
       <c r="K206">
-        <f t="shared" ref="K206:K231" si="4">(F206/F205)-1</f>
+        <f t="shared" ref="K206:K231" si="8">(F206/F205)-1</f>
         <v>-2.1474414251417051E-2</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L206">
+        <f t="shared" si="7"/>
+        <v>-2.170834455879958E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="d">
         <v>2018-11-21</v>
       </c>
@@ -8084,11 +8906,15 @@
         <v>10619600</v>
       </c>
       <c r="K207">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-7.4688317115567671E-3</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L207">
+        <f t="shared" si="7"/>
+        <v>-7.496863096809846E-3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="d">
         <v>2018-11-23</v>
       </c>
@@ -8111,11 +8937,15 @@
         <v>6488400</v>
       </c>
       <c r="K208">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-9.197280756016335E-3</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L208">
+        <f t="shared" si="7"/>
+        <v>-9.2398368773764453E-3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="d">
         <v>2018-11-26</v>
       </c>
@@ -8138,11 +8968,15 @@
         <v>13948300</v>
       </c>
       <c r="K209">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2.4472583909632029E-2</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L209">
+        <f t="shared" si="7"/>
+        <v>2.4177927879630377E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="d">
         <v>2018-11-27</v>
       </c>
@@ -8165,11 +8999,15 @@
         <v>9238200</v>
       </c>
       <c r="K210">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.2101398409941648E-3</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L210">
+        <f t="shared" si="7"/>
+        <v>4.2013019992700358E-3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="d">
         <v>2018-11-28</v>
       </c>
@@ -8192,11 +9030,15 @@
         <v>13977300</v>
       </c>
       <c r="K211">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1119243276485058E-2</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L211">
+        <f t="shared" si="7"/>
+        <v>1.1057878955161112E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="d">
         <v>2018-11-29</v>
       </c>
@@ -8219,11 +9061,15 @@
         <v>11144300</v>
       </c>
       <c r="K212">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-7.9322746362493479E-3</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L212">
+        <f t="shared" si="7"/>
+        <v>-7.9639024916205465E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="d">
         <v>2018-11-30</v>
       </c>
@@ -8246,11 +9092,15 @@
         <v>18652700</v>
       </c>
       <c r="K213">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.0267150900574951E-2</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L213">
+        <f t="shared" si="7"/>
+        <v>1.0214801719818581E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="d">
         <v>2018-12-03</v>
       </c>
@@ -8273,11 +9123,15 @@
         <v>16034500</v>
       </c>
       <c r="K214">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9.4432388347611695E-3</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L214">
+        <f t="shared" si="7"/>
+        <v>9.3989301813010347E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="d">
         <v>2018-12-04</v>
       </c>
@@ -8300,11 +9154,15 @@
         <v>23555900</v>
       </c>
       <c r="K215">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-4.4636416512855659E-2</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L215">
+        <f t="shared" si="7"/>
+        <v>-4.566329526189257E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="d">
         <v>2018-12-06</v>
       </c>
@@ -8327,11 +9185,15 @@
         <v>27213900</v>
       </c>
       <c r="K216">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1.9024499805955997E-2</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L216">
+        <f t="shared" si="7"/>
+        <v>-1.9207794046635397E-2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="d">
         <v>2018-12-07</v>
       </c>
@@ -8354,11 +9216,15 @@
         <v>19248600</v>
       </c>
       <c r="K217">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1.8062601608510365E-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L217">
+        <f t="shared" si="7"/>
+        <v>-1.8227721751900315E-2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="d">
         <v>2018-12-10</v>
       </c>
@@ -8381,11 +9247,15 @@
         <v>23636400</v>
       </c>
       <c r="K218">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1.868524810993355E-2</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L218">
+        <f t="shared" si="7"/>
+        <v>-1.8862022875380639E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="d">
         <v>2018-12-11</v>
       </c>
@@ -8408,11 +9278,15 @@
         <v>16860700</v>
       </c>
       <c r="K219">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-9.7671297050234696E-3</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L219">
+        <f t="shared" si="7"/>
+        <v>-9.8151409938026339E-3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="d">
         <v>2018-12-12</v>
       </c>
@@ -8435,11 +9309,15 @@
         <v>22621500</v>
       </c>
       <c r="K220">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6.4759516054251343E-3</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L220">
+        <f t="shared" si="7"/>
+        <v>6.4550727227715527E-3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="d">
         <v>2018-12-13</v>
       </c>
@@ -8462,11 +9340,15 @@
         <v>17250900</v>
       </c>
       <c r="K221">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9.8989132674720537E-4</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L221">
+        <f t="shared" si="7"/>
+        <v>9.8940170741446815E-4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="d">
         <v>2018-12-14</v>
       </c>
@@ -8489,11 +9371,15 @@
         <v>19879500</v>
       </c>
       <c r="K222">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-8.2079891978407149E-3</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L222">
+        <f t="shared" si="7"/>
+        <v>-8.2418602104453436E-3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="d">
         <v>2018-12-17</v>
       </c>
@@ -8516,11 +9402,15 @@
         <v>25113500</v>
       </c>
       <c r="K223">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1.2763076816738606E-2</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L223">
+        <f t="shared" si="7"/>
+        <v>-1.2845224602509336E-2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="d">
         <v>2018-12-18</v>
       </c>
@@ -8543,11 +9433,15 @@
         <v>20837200</v>
       </c>
       <c r="K224">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-4.7469745565764665E-3</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L224">
+        <f t="shared" si="7"/>
+        <v>-4.7582772234637518E-3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="d">
         <v>2018-12-19</v>
       </c>
@@ -8570,11 +9464,15 @@
         <v>28767900</v>
       </c>
       <c r="K225">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-1.268518949364994E-2</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L225">
+        <f t="shared" si="7"/>
+        <v>-1.2766333457952164E-2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="d">
         <v>2018-12-20</v>
       </c>
@@ -8597,11 +9495,15 @@
         <v>31825200</v>
       </c>
       <c r="K226">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-8.6340346609964369E-3</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L226">
+        <f t="shared" si="7"/>
+        <v>-8.6715238830682457E-3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="d">
         <v>2018-12-21</v>
       </c>
@@ -8624,11 +9526,15 @@
         <v>41313900</v>
       </c>
       <c r="K227">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-2.3639142832713955E-2</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L227">
+        <f t="shared" si="7"/>
+        <v>-2.3923030198412031E-2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="d">
         <v>2018-12-24</v>
       </c>
@@ -8651,11 +9557,15 @@
         <v>17009300</v>
       </c>
       <c r="K228">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-2.1556739523185264E-2</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L228">
+        <f t="shared" si="7"/>
+        <v>-2.1792480054339598E-2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="d">
         <v>2018-12-26</v>
       </c>
@@ -8678,11 +9588,15 @@
         <v>22542900</v>
       </c>
       <c r="K229">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.1458719788054266E-2</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L229">
+        <f t="shared" si="7"/>
+        <v>4.0622345588265461E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="d">
         <v>2018-12-27</v>
       </c>
@@ -8705,11 +9619,15 @@
         <v>20304700</v>
       </c>
       <c r="K230">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1254562162223758E-2</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L230">
+        <f t="shared" si="7"/>
+        <v>1.1191700789261945E-2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="d">
         <v>2018-12-28</v>
       </c>
@@ -8732,11 +9650,15 @@
         <v>17963300</v>
       </c>
       <c r="K231">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-2.1639273113727153E-3</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L231">
+        <f t="shared" si="7"/>
+        <v>-2.1662719851569161E-3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E232" s="3" t="s">
         <v>8</v>
       </c>
@@ -8750,6 +9672,10 @@
       <c r="K232" s="4">
         <f>_xlfn.STDEV.S(K3:K231)</f>
         <v>1.437042735085395E-2</v>
+      </c>
+      <c r="L232" s="4">
+        <f>_xlfn.STDEV.S(L3:L231)</f>
+        <v>1.4405585766155913E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>